<commit_message>
Ran workflow osw files, generated csv, re-generated excel files
Confimred that updated scripts using combined CSV file runs fine.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14497,7 +14497,7 @@
         <v>111</v>
       </c>
       <c r="B52" s="5">
-        <v>0.00026315789473684215</v>
+        <v>0.000263158</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -14512,7 +14512,7 @@
         <v>112</v>
       </c>
       <c r="B53" s="5">
-        <v>0.0003289473684210526</v>
+        <v>0.000328947</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -14527,7 +14527,7 @@
         <v>113</v>
       </c>
       <c r="B54" s="243">
-        <v>0.00012988683127572017</v>
+        <v>0.000129887</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -14542,7 +14542,7 @@
         <v>114</v>
       </c>
       <c r="B55" s="242">
-        <v>3.384232185401776e-08</v>
+        <v>3.38423e-08</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -14557,7 +14557,7 @@
         <v>115</v>
       </c>
       <c r="B56" s="5">
-        <v>0.00013208658219623134</v>
+        <v>0.000132087</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -14572,7 +14572,7 @@
         <v>116</v>
       </c>
       <c r="B57" s="5">
-        <v>0.00012626570283734027</v>
+        <v>0.000126266</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -14587,7 +14587,7 @@
         <v>117</v>
       </c>
       <c r="B58" s="5">
-        <v>0.00012968377734459607</v>
+        <v>0.000129684</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -14602,7 +14602,7 @@
         <v>118</v>
       </c>
       <c r="B59" s="5">
-        <v>0.00012626570283734027</v>
+        <v>0.000126266</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -14617,7 +14617,7 @@
         <v>119</v>
       </c>
       <c r="B60" s="5">
-        <v>0.00017858593242365173</v>
+        <v>0.000178586</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -14632,7 +14632,7 @@
         <v>120</v>
       </c>
       <c r="B61" s="5">
-        <v>0.00016887318605154862</v>
+        <v>0.000168873</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -14647,7 +14647,7 @@
         <v>121</v>
       </c>
       <c r="B62" s="5">
-        <v>0.0001469095191682911</v>
+        <v>0.00014691</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -14725,7 +14725,7 @@
         <v>116</v>
       </c>
       <c r="B68" s="244">
-        <v>433.3333333333333</v>
+        <v>433.333</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -14740,7 +14740,7 @@
         <v>117</v>
       </c>
       <c r="B69" s="244">
-        <v>172.22222222222223</v>
+        <v>172.222</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -14755,7 +14755,7 @@
         <v>118</v>
       </c>
       <c r="B70" s="244">
-        <v>475.0</v>
+        <v>475</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -14770,7 +14770,7 @@
         <v>119</v>
       </c>
       <c r="B71" s="244">
-        <v>294.44444444444446</v>
+        <v>294.444</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
@@ -14785,7 +14785,7 @@
         <v>120</v>
       </c>
       <c r="B72" s="244">
-        <v>277.77777777777777</v>
+        <v>277.778</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -14800,7 +14800,7 @@
         <v>121</v>
       </c>
       <c r="B73" s="244">
-        <v>483.33333333333337</v>
+        <v>483.333</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -14878,7 +14878,7 @@
         <v>119</v>
       </c>
       <c r="B79" s="13">
-        <v>20.000271801908607</v>
+        <v>20.0003</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -14893,7 +14893,7 @@
         <v>120</v>
       </c>
       <c r="B80" s="13">
-        <v>18.536820123570024</v>
+        <v>18.5368</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -14908,7 +14908,7 @@
         <v>121</v>
       </c>
       <c r="B81" s="13">
-        <v>15.3750299090923</v>
+        <v>15.375</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -14986,7 +14986,7 @@
         <v>119</v>
       </c>
       <c r="B87" s="13">
-        <v>20.001408372470884</v>
+        <v>20.0014</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="11"/>
@@ -15001,7 +15001,7 @@
         <v>120</v>
       </c>
       <c r="B88" s="13">
-        <v>20.00140801600231</v>
+        <v>20.0014</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="11"/>
@@ -15016,7 +15016,7 @@
         <v>121</v>
       </c>
       <c r="B89" s="13">
-        <v>20.001411402225735</v>
+        <v>20.0014</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
@@ -15094,7 +15094,7 @@
         <v>119</v>
       </c>
       <c r="B95" s="13">
-        <v>19.9999999999998</v>
+        <v>20</v>
       </c>
       <c r="C95" s="10"/>
       <c r="D95" s="11"/>
@@ -15109,7 +15109,7 @@
         <v>120</v>
       </c>
       <c r="B96" s="13">
-        <v>14.999999999999822</v>
+        <v>15</v>
       </c>
       <c r="C96" s="10"/>
       <c r="D96" s="11"/>
@@ -15124,7 +15124,7 @@
         <v>121</v>
       </c>
       <c r="B97" s="13">
-        <v>1.8576146684294725</v>
+        <v>1.85761</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>

</xml_diff>

<commit_message>
OpenStudio 2.5.0 EnergyPlus 8.9 run
I need to look through heating and cooling results before I push to master and create a release.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -10824,7 +10824,6 @@
     <row r="7" spans="2:2" s="1" customFormat="1" ht="15">
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="15"/>
     <row r="9" spans="1:2" s="1" customFormat="1" ht="15">
       <c r="A9" s="1" t="s">
         <v>20</v>
@@ -16333,7 +16332,6 @@
       <c r="C20" s="119"/>
       <c r="D20" s="119"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="22" spans="1:4" customFormat="false" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="129" t="s">
         <v>68</v>
@@ -16814,7 +16812,6 @@
       </c>
       <c r="E29" s="383"/>
     </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:F1"/>
@@ -24805,7 +24802,6 @@
     <row r="6" spans="5:5" customFormat="false" ht="15">
       <c r="E6" s="101"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="9" spans="1:8" customFormat="false" ht="13.5" thickBot="1">
       <c r="A9" s="94" t="s">
         <v>23</v>
@@ -25165,7 +25161,6 @@
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
     </row>
-    <row r="25" spans="1:13" ht="13.5" thickBot="1"/>
     <row r="26" spans="1:13" customFormat="false" ht="15">
       <c r="A26" s="33"/>
       <c r="B26" s="63" t="str">
@@ -25912,7 +25907,6 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:5" customFormat="false" ht="15.75">
       <c r="A43" s="49"/>
       <c r="B43" s="71" t="str">
@@ -26111,7 +26105,6 @@
     <row r="54" spans="1:1" customFormat="false">
       <c r="A54" s="36"/>
     </row>
-    <row r="55" spans="1:13" ht="13.5" thickBot="1"/>
     <row r="56" spans="1:13" customFormat="false" ht="15.75">
       <c r="A56" s="49"/>
       <c r="B56" s="71" t="str">

</xml_diff>

<commit_message>
updating general info in Excel files
Release dates and versions for OS and EP were out of date, as was the submission date.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 8.8.0</v>
+        <v>EnergyPlus 8.9.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>9/30/2017</v>
+        <v>3/29/2018</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>10/04/2017</v>
+        <v>4/04/2018</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
OpenSudio 270 EP 901 release run results
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 8.9.0</v>
+        <v>EnergyPlus 9.0.1</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>3/29/2018</v>
+        <v>10/9/2018</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>4/04/2018</v>
+        <v>10/21/2018</v>
       </c>
       <c r="K5" s="109"/>
     </row>
@@ -14085,7 +14085,7 @@
         <v>114</v>
       </c>
       <c r="B23" s="13">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -14313,7 +14313,7 @@
         <v>114</v>
       </c>
       <c r="B39" s="13">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -14541,7 +14541,7 @@
         <v>114</v>
       </c>
       <c r="B55" s="242">
-        <v>3.38423e-08</v>
+        <v>3.72266e-07</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>

</xml_diff>

<commit_message>
progress update on code to gather historical values
@myoldmopar Note, initial run for OS 2.8 EP 9.1 have some holes in CE data used in charts 16.5.2 43 through 52 on 3B. I'm looking into that now, probably an issue with SQL query.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 9.0.1</v>
+        <v>EnergyPlus 9.1.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>10/9/2018</v>
+        <v>3/31/2019</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>10/21/2018</v>
+        <v>04/15/2019</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
first pass at 290 run
Note that something happened on Mac with RubyXL since last run that was creating issue, so I ran on Windows machine. The error didn't come up there.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 9.1.0</v>
+        <v>EnergyPlus 9.2.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>3/31/2019</v>
+        <v>9/27/2019</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Updating output variables for EnergyPlu 9.4 and initial results
Will re-run and and zip files when final OpenStudio Release is out.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 9.3.0</v>
+        <v>EnergyPlus 9.4.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/27/2020</v>
+        <v>09/29/2020</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>05/19/2020</v>
+        <v>10/01/2020</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
initial results with alpha OS32 and EP95
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 9.4.0</v>
+        <v>EnergyPlus 9.5.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>09/29/2020</v>
+        <v>03/31/2021</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>10/19/2020</v>
+        <v>05/08/2021</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
run with final release
note no changes in histiral csv files from last run other than date. so no changes in results that make it to your data in Excel files.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/31/2021</v>
+        <v>03/30/2021</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>05/08/2021</v>
+        <v>05/04/2021</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
Updated run with temp EP installer
it addresses weather file parsing.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 9.5.0</v>
+        <v>EnergyPlus 9.6.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/30/2021</v>
+        <v>09/23/21</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>05/04/2021</v>
+        <v>01/20/2022</v>
       </c>
       <c r="K5" s="109"/>
     </row>
@@ -14160,7 +14160,7 @@
         <v>119</v>
       </c>
       <c r="B28" s="13">
-        <v>43.034</v>
+        <v>43.002</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -14175,7 +14175,7 @@
         <v>120</v>
       </c>
       <c r="B29" s="13">
-        <v>40.742</v>
+        <v>40.71</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -14190,7 +14190,7 @@
         <v>121</v>
       </c>
       <c r="B30" s="13">
-        <v>35.815</v>
+        <v>35.789</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -14388,7 +14388,7 @@
         <v>119</v>
       </c>
       <c r="B44" s="13">
-        <v>52.77</v>
+        <v>52.73</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -14403,7 +14403,7 @@
         <v>120</v>
       </c>
       <c r="B45" s="13">
-        <v>49.9</v>
+        <v>49.86</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -14418,7 +14418,7 @@
         <v>121</v>
       </c>
       <c r="B46" s="13">
-        <v>43.42</v>
+        <v>43.38</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -14616,7 +14616,7 @@
         <v>119</v>
       </c>
       <c r="B60" s="5">
-        <v>0.000178586</v>
+        <v>0.000178451</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -14631,7 +14631,7 @@
         <v>120</v>
       </c>
       <c r="B61" s="5">
-        <v>0.000168873</v>
+        <v>0.000168738</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -14646,7 +14646,7 @@
         <v>121</v>
       </c>
       <c r="B62" s="5">
-        <v>0.000146943</v>
+        <v>0.000146808</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -14892,7 +14892,7 @@
         <v>120</v>
       </c>
       <c r="B80" s="13">
-        <v>18.5368</v>
+        <v>18.5369</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -14907,7 +14907,7 @@
         <v>121</v>
       </c>
       <c r="B81" s="13">
-        <v>15.3747</v>
+        <v>15.3792</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>

</xml_diff>

<commit_message>
final results for OS3.4 EP22.1
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -13776,7 +13776,7 @@
         <v>39</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 9.6.0</v>
+        <v>EnergyPlus 22.1</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>09/23/21</v>
+        <v>03/29/22</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>01/20/2022</v>
+        <v>05/05/2022</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
Progress update with rc OS installer
Few envelope values that aren't coming through, likely change in sql query in E+. Also few CE value changes to investigate.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 22.1</v>
+        <v>EnergyPlus 22.2</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/29/22</v>
+        <v>09/27/22</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14322,7 +14322,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>05/27/2022</v>
+        <v>11/03/2022</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
update version and results
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 23.1</v>
+        <v>EnergyPlus 23.2</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/28/23</v>
+        <v>09/28/2023</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14322,7 +14322,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>05/09/2023</v>
+        <v>11/18/2023</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
Results for EnergyPlus 23.2 and OpenStudio 3.7
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 23.1</v>
+        <v>EnergyPlus 23.2</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/28/2023</v>
+        <v>09/28/2023</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14322,7 +14322,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>11/05/2024</v>
+        <v>11/06/2024</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
EnergyPlus 24.1 and OpenStudio 3.8 results
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>09/28/2023</v>
+        <v>03/28/2024</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14663,7 +14663,7 @@
         <v>118</v>
       </c>
       <c r="B29" s="13">
-        <v>40.742</v>
+        <v>40.743</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -14678,7 +14678,7 @@
         <v>119</v>
       </c>
       <c r="B30" s="13">
-        <v>35.815</v>
+        <v>35.821</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -15380,7 +15380,7 @@
         <v>118</v>
       </c>
       <c r="B80" s="13">
-        <v>18.5368</v>
+        <v>18.537</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -15395,7 +15395,7 @@
         <v>119</v>
       </c>
       <c r="B81" s="13">
-        <v>15.3747</v>
+        <v>15.3752</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -15611,7 +15611,7 @@
         <v>119</v>
       </c>
       <c r="B97" s="13">
-        <v>1.85761</v>
+        <v>1.85752</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>

</xml_diff>

<commit_message>
updating final results and release dates for E+ 24.2.1 and OS 3.9.0
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 24.2</v>
+        <v>EnergyPlus 24.2.1</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>03/28/2024</v>
+        <v>10/03/24</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14322,7 +14322,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>11/06/2024</v>
+        <v>11/15/2024</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
EnergyPlus 25.1 OpenStudio 3.10 runs and updated historical Excel file
still had to copy and paste yourdata in 3a to get figures to render.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4.xlsx
+++ b/results/RESULTS5-4.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>EnergyPlus 24.2.1</v>
+        <v>EnergyPlus 25.1.0 , Bug Fix Edition</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>10/03/24</v>
+        <v>05/28/25</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14322,7 +14322,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>11/15/2024</v>
+        <v>06/18/2025</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>